<commit_message>
playing with CA allele freqs
</commit_message>
<xml_diff>
--- a/CA_related/pro_vs_arg.xlsx
+++ b/CA_related/pro_vs_arg.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csengepetak/Desktop/WGS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csengeswork/Desktop/WGS/CA_related/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888E0AD-4380-C74C-BCA8-574374307C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF689323-3191-E441-9443-95D5ACA2D3D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{12F6A034-2461-AB4D-AC01-B69E2FAD47A7}"/>
+    <workbookView xWindow="10660" yWindow="1880" windowWidth="28800" windowHeight="18000" xr2:uid="{12F6A034-2461-AB4D-AC01-B69E2FAD47A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4798,7 +4798,7 @@
   <dimension ref="A1:U89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5582,7 +5582,7 @@
         <v>40</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:H44" si="2">SUM(C39,C41)</f>
+        <f t="shared" ref="C44:G44" si="2">SUM(C39,C41)</f>
         <v>40</v>
       </c>
       <c r="D44">

</xml_diff>